<commit_message>
Changes on security Issues
</commit_message>
<xml_diff>
--- a/Forms.xlsx
+++ b/Forms.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="133">
   <si>
     <t>PLANILHA DE INFORMAÇÕES GERAIS</t>
   </si>
@@ -272,6 +272,36 @@
   </si>
   <si>
     <t>Sgt. J. Alves</t>
+  </si>
+  <si>
+    <t>0346.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Jonathan</t>
+  </si>
+  <si>
+    <t>0518.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Michel</t>
+  </si>
+  <si>
+    <t>0349.9/2023</t>
+  </si>
+  <si>
+    <t>St. Andreyer</t>
+  </si>
+  <si>
+    <t>0362.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Andrelino</t>
+  </si>
+  <si>
+    <t>0361.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. R. Soares</t>
   </si>
   <si>
     <t>INFORMAÇÕES DAS VÍTIMAS</t>
@@ -1687,7 +1717,137 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="6"/>
+      <c r="A39" s="6">
+        <v>45102.08596229166</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1031813.0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6">
+        <v>45106.55609578703</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="3">
+        <v>9808655.0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6">
+        <v>45107.06797804398</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="3">
+        <v>9901221.0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6">
+        <v>45112.384029444445</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="3">
+        <v>9901280.0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6">
+        <v>45116.533558807874</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="3">
+        <v>136512.0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>17.0</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1722,7 +1882,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
@@ -1733,37 +1893,37 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
@@ -2174,33 +2334,73 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="6"/>
-      <c r="B40" s="3"/>
+      <c r="A40" s="6">
+        <v>45102.08635333333</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="3">
+        <v>136534.0</v>
+      </c>
     </row>
     <row r="41">
-      <c r="K41" s="3"/>
-      <c r="L41" s="9"/>
+      <c r="A41" s="6">
+        <v>45106.557955208336</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="3">
+        <v>137792.0</v>
+      </c>
     </row>
     <row r="42">
-      <c r="L42" s="9"/>
+      <c r="A42" s="6">
+        <v>45107.06833642361</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="3">
+        <v>136528.0</v>
+      </c>
     </row>
     <row r="43">
-      <c r="K43" s="10"/>
-      <c r="L43" s="9"/>
+      <c r="A43" s="6">
+        <v>45112.38436751158</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="3">
+        <v>136507.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="L44" s="9"/>
+      <c r="A44" s="6">
+        <v>45116.533809120374</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="3">
+        <v>136512.0</v>
+      </c>
     </row>
     <row r="45">
-      <c r="L45" s="9"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="3"/>
     </row>
     <row r="46">
+      <c r="K46" s="3"/>
       <c r="L46" s="9"/>
     </row>
     <row r="47">
       <c r="L47" s="9"/>
     </row>
     <row r="48">
+      <c r="K48" s="10"/>
       <c r="L48" s="9"/>
     </row>
     <row r="49">
@@ -2475,6 +2675,21 @@
     </row>
     <row r="139">
       <c r="L139" s="9"/>
+    </row>
+    <row r="140">
+      <c r="L140" s="9"/>
+    </row>
+    <row r="141">
+      <c r="L141" s="9"/>
+    </row>
+    <row r="142">
+      <c r="L142" s="9"/>
+    </row>
+    <row r="143">
+      <c r="L143" s="9"/>
+    </row>
+    <row r="144">
+      <c r="L144" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2510,7 +2725,7 @@
   <sheetData>
     <row r="1" ht="31.5" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -2521,34 +2736,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
@@ -2556,7 +2771,7 @@
         <v>44457.81127759259</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C3" s="3">
         <v>5.63</v>
@@ -2565,16 +2780,16 @@
         <v>9.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
@@ -2606,7 +2821,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2">
@@ -2617,28 +2832,28 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correções por erro na versão
</commit_message>
<xml_diff>
--- a/Forms.xlsx
+++ b/Forms.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="133">
   <si>
     <t>PLANILHA DE INFORMAÇÕES GERAIS</t>
   </si>
@@ -290,6 +290,18 @@
   </si>
   <si>
     <t>St. Andreyer</t>
+  </si>
+  <si>
+    <t>0362.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Andrelino</t>
+  </si>
+  <si>
+    <t>0361.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. R. Soares</t>
   </si>
   <si>
     <t>INFORMAÇÕES DAS VÍTIMAS</t>
@@ -1783,7 +1795,59 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="6"/>
+      <c r="A42" s="6">
+        <v>45112.384029444445</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="3">
+        <v>9901280.0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6">
+        <v>45116.533558807874</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="3">
+        <v>136512.0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>17.0</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1818,7 +1882,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
@@ -1829,37 +1893,37 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
@@ -2303,24 +2367,40 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="6"/>
-      <c r="B43" s="3"/>
+      <c r="A43" s="6">
+        <v>45112.38436751158</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="3">
+        <v>136507.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="K44" s="3"/>
-      <c r="L44" s="9"/>
+      <c r="A44" s="6">
+        <v>45116.533809120374</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="3">
+        <v>136512.0</v>
+      </c>
     </row>
     <row r="45">
-      <c r="L45" s="9"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="3"/>
     </row>
     <row r="46">
-      <c r="K46" s="10"/>
+      <c r="K46" s="3"/>
       <c r="L46" s="9"/>
     </row>
     <row r="47">
       <c r="L47" s="9"/>
     </row>
     <row r="48">
+      <c r="K48" s="10"/>
       <c r="L48" s="9"/>
     </row>
     <row r="49">
@@ -2604,6 +2684,12 @@
     </row>
     <row r="142">
       <c r="L142" s="9"/>
+    </row>
+    <row r="143">
+      <c r="L143" s="9"/>
+    </row>
+    <row r="144">
+      <c r="L144" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2639,7 +2725,7 @@
   <sheetData>
     <row r="1" ht="31.5" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -2650,34 +2736,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
@@ -2685,7 +2771,7 @@
         <v>44457.81127759259</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C3" s="3">
         <v>5.63</v>
@@ -2694,16 +2780,16 @@
         <v>9.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
@@ -2735,7 +2821,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2">
@@ -2746,28 +2832,28 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit para finalizar AddLocal
</commit_message>
<xml_diff>
--- a/Forms.xlsx
+++ b/Forms.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="204">
   <si>
     <t>PLANILHA DE INFORMAÇÕES GERAIS</t>
   </si>
@@ -290,6 +290,231 @@
   </si>
   <si>
     <t>St. Andreyer</t>
+  </si>
+  <si>
+    <t>0362.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Andrelino</t>
+  </si>
+  <si>
+    <t>0361.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. R. Soares</t>
+  </si>
+  <si>
+    <t>0593.9/2023</t>
+  </si>
+  <si>
+    <t>Sd. Valdeci</t>
+  </si>
+  <si>
+    <t>0365.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Rommel</t>
+  </si>
+  <si>
+    <t>0421.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Felipino</t>
+  </si>
+  <si>
+    <t>0439.9/2023</t>
+  </si>
+  <si>
+    <t>Sd. Farias</t>
+  </si>
+  <si>
+    <t>0427.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Sérgio Torres</t>
+  </si>
+  <si>
+    <t>0457.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Freitas</t>
+  </si>
+  <si>
+    <t>0473.9/2023</t>
+  </si>
+  <si>
+    <t>xxxxxxxxx</t>
+  </si>
+  <si>
+    <t>000000000</t>
+  </si>
+  <si>
+    <t>0481.9/2023</t>
+  </si>
+  <si>
+    <t>ccccc</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>0487.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Petrunilo</t>
+  </si>
+  <si>
+    <t>0490.9/2023</t>
+  </si>
+  <si>
+    <t>Sd. Geandson</t>
+  </si>
+  <si>
+    <t>0507.9/2023</t>
+  </si>
+  <si>
+    <t>dddddddd</t>
+  </si>
+  <si>
+    <t>0515.9/2023</t>
+  </si>
+  <si>
+    <t>0542.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Jenilson Tavares</t>
+  </si>
+  <si>
+    <t>0556.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Adriano</t>
+  </si>
+  <si>
+    <t>0555.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Janio</t>
+  </si>
+  <si>
+    <t>0563.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Denildo</t>
+  </si>
+  <si>
+    <t>0567.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Willamis</t>
+  </si>
+  <si>
+    <t>0600.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. José Brito</t>
+  </si>
+  <si>
+    <t>0545.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Danilo Gomes</t>
+  </si>
+  <si>
+    <t>0682.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Telmo</t>
+  </si>
+  <si>
+    <t>0847.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Ralph</t>
+  </si>
+  <si>
+    <t>0639.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Edmilson</t>
+  </si>
+  <si>
+    <t>0642.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. R. Junior</t>
+  </si>
+  <si>
+    <t>0649.9/2023</t>
+  </si>
+  <si>
+    <t>Sd. João Alves</t>
+  </si>
+  <si>
+    <t>0651.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Amanda</t>
+  </si>
+  <si>
+    <t>0873.9/2023</t>
+  </si>
+  <si>
+    <t>Sd. Talyta</t>
+  </si>
+  <si>
+    <t>0684.9/2023</t>
+  </si>
+  <si>
+    <t>Valder Vieira</t>
+  </si>
+  <si>
+    <t>0687.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Flávia</t>
+  </si>
+  <si>
+    <t>0966.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Nominando</t>
+  </si>
+  <si>
+    <t>0692.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Gaspar</t>
+  </si>
+  <si>
+    <t>0824.9/2023</t>
+  </si>
+  <si>
+    <t>Sd. João França</t>
+  </si>
+  <si>
+    <t>0830.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Gerdiano</t>
+  </si>
+  <si>
+    <t>0831.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Nascimento</t>
+  </si>
+  <si>
+    <t>0833.9/2023</t>
+  </si>
+  <si>
+    <t>Sd. Rayara</t>
+  </si>
+  <si>
+    <t>0843.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Rildo</t>
   </si>
   <si>
     <t>INFORMAÇÕES DAS VÍTIMAS</t>
@@ -1783,7 +2008,956 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="6"/>
+      <c r="A42" s="6">
+        <v>45112.384029444445</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="3">
+        <v>9901280.0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6">
+        <v>45116.533558807874</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="3">
+        <v>136512.0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>17.0</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6">
+        <v>45116.83300459491</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1257757.0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6">
+        <v>45126.42473561343</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1179136.0</v>
+      </c>
+      <c r="G45" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6">
+        <v>45126.60111041667</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1163272.0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6">
+        <v>45126.67929339121</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1253131.0</v>
+      </c>
+      <c r="G47" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6">
+        <v>45126.9445546412</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1109278.0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>19.0</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6">
+        <v>45173.86764729167</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1160915.0</v>
+      </c>
+      <c r="G49" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6">
+        <v>45178.71452008102</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G50" s="3">
+        <v>99.0</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6">
+        <v>45179.51289844907</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G51" s="3">
+        <v>99.0</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6">
+        <v>45179.51297991898</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G52" s="3">
+        <v>99.0</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6">
+        <v>45179.600141828705</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F53" s="3">
+        <v>9902473.0</v>
+      </c>
+      <c r="G53" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6">
+        <v>45181.37111256944</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F54" s="3">
+        <v>1257854.0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6">
+        <v>45182.013505428244</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F55" s="3">
+        <v>99.0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>99.0</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="6">
+        <v>45188.886567939815</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1257854.0</v>
+      </c>
+      <c r="G56" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6">
+        <v>45189.018730717595</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1111132.0</v>
+      </c>
+      <c r="G57" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="6">
+        <v>45190.81339351852</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F58" s="3">
+        <v>1104462.0</v>
+      </c>
+      <c r="G58" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6">
+        <v>45190.96886771991</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F59" s="3">
+        <v>9808272.0</v>
+      </c>
+      <c r="G59" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="6">
+        <v>45194.55907579861</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F60" s="3">
+        <v>9808272.0</v>
+      </c>
+      <c r="G60" s="3">
+        <v>17.0</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6">
+        <v>45194.96895946759</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F61" s="3">
+        <v>1078755.0</v>
+      </c>
+      <c r="G61" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="6">
+        <v>45198.853209085646</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F62" s="3">
+        <v>1102818.0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6">
+        <v>45202.94848186342</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1164392.0</v>
+      </c>
+      <c r="G63" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="6">
+        <v>45205.807649375</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1076027.0</v>
+      </c>
+      <c r="G64" s="3">
+        <v>17.0</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6">
+        <v>45208.340232372684</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F65" s="3">
+        <v>140936.0</v>
+      </c>
+      <c r="G65" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6">
+        <v>45209.75365520833</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F66" s="3">
+        <v>138300.0</v>
+      </c>
+      <c r="G66" s="3">
+        <v>26.0</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6">
+        <v>45218.37707783565</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1056048.0</v>
+      </c>
+      <c r="G67" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="6">
+        <v>45218.851198854165</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F68" s="3">
+        <v>1205382.0</v>
+      </c>
+      <c r="G68" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6">
+        <v>45220.87860931713</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F69" s="3">
+        <v>1155520.0</v>
+      </c>
+      <c r="G69" s="3">
+        <v>17.0</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="6">
+        <v>45228.08590427083</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1251856.0</v>
+      </c>
+      <c r="G70" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6">
+        <v>45250.504648055554</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F71" s="3">
+        <v>1164414.0</v>
+      </c>
+      <c r="G71" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="6">
+        <v>45250.82394229167</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F72" s="3">
+        <v>1047973.0</v>
+      </c>
+      <c r="G72" s="3">
+        <v>26.0</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6">
+        <v>45260.361299965276</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1103920.0</v>
+      </c>
+      <c r="G73" s="3">
+        <v>111111.0</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="6">
+        <v>45260.991132361116</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1158155.0</v>
+      </c>
+      <c r="G74" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6">
+        <v>45261.77620087963</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F75" s="3">
+        <v>1205250.0</v>
+      </c>
+      <c r="G75" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="6">
+        <v>45263.71817685185</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F76" s="3">
+        <v>1078917.0</v>
+      </c>
+      <c r="G76" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6">
+        <v>45268.47325917824</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F77" s="3">
+        <v>9302930.0</v>
+      </c>
+      <c r="G77" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="6">
+        <v>45268.58561106482</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F78" s="3">
+        <v>1261240.0</v>
+      </c>
+      <c r="G78" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="6">
+        <v>45271.80265429398</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F79" s="3">
+        <v>9307575.0</v>
+      </c>
+      <c r="G79" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1818,7 +2992,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>92</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2">
@@ -1829,37 +3003,37 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>93</v>
+        <v>168</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>94</v>
+        <v>169</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>170</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>97</v>
+        <v>172</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>98</v>
+        <v>173</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>99</v>
+        <v>174</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>102</v>
+        <v>177</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>103</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3">
@@ -2303,129 +3477,425 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="6"/>
-      <c r="B43" s="3"/>
+      <c r="A43" s="6">
+        <v>45112.38436751158</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="3">
+        <v>136507.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="K44" s="3"/>
-      <c r="L44" s="9"/>
+      <c r="A44" s="6">
+        <v>45116.533809120374</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="3">
+        <v>136512.0</v>
+      </c>
     </row>
     <row r="45">
-      <c r="L45" s="9"/>
+      <c r="A45" s="6">
+        <v>45116.83355563658</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="3">
+        <v>137995.0</v>
+      </c>
     </row>
     <row r="46">
-      <c r="K46" s="10"/>
-      <c r="L46" s="9"/>
+      <c r="A46" s="6">
+        <v>45126.42507981481</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="3">
+        <v>136514.0</v>
+      </c>
     </row>
     <row r="47">
-      <c r="L47" s="9"/>
+      <c r="A47" s="6">
+        <v>45126.60159921296</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="3">
+        <v>136999.0</v>
+      </c>
     </row>
     <row r="48">
-      <c r="L48" s="9"/>
+      <c r="A48" s="6">
+        <v>45126.67963648148</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="3">
+        <v>137281.0</v>
+      </c>
     </row>
     <row r="49">
-      <c r="L49" s="9"/>
+      <c r="A49" s="6">
+        <v>45126.94496903935</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="3">
+        <v>137009.0</v>
+      </c>
     </row>
     <row r="50">
-      <c r="L50" s="9"/>
+      <c r="A50" s="6">
+        <v>45173.86704675926</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="3">
+        <v>137295.0</v>
+      </c>
     </row>
     <row r="51">
-      <c r="L51" s="9"/>
+      <c r="A51" s="6">
+        <v>45178.71479252315</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="3">
+        <v>137380.0</v>
+      </c>
     </row>
     <row r="52">
-      <c r="L52" s="9"/>
+      <c r="A52" s="6">
+        <v>45179.51325885417</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="3">
+        <v>137375.0</v>
+      </c>
     </row>
     <row r="53">
-      <c r="L53" s="9"/>
+      <c r="A53" s="6">
+        <v>45179.600456898144</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="3">
+        <v>137305.0</v>
+      </c>
     </row>
     <row r="54">
-      <c r="L54" s="9"/>
+      <c r="A54" s="6">
+        <v>45181.37158980324</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="3">
+        <v>137370.0</v>
+      </c>
     </row>
     <row r="55">
-      <c r="L55" s="9"/>
+      <c r="A55" s="6">
+        <v>45182.01385804398</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="3">
+        <v>137806.0</v>
+      </c>
     </row>
     <row r="56">
-      <c r="L56" s="9"/>
+      <c r="A56" s="6">
+        <v>45188.88684202546</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="3">
+        <v>137804.0</v>
+      </c>
     </row>
     <row r="57">
-      <c r="L57" s="9"/>
+      <c r="A57" s="6">
+        <v>45189.019096793985</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="3">
+        <v>137788.0</v>
+      </c>
     </row>
     <row r="58">
-      <c r="L58" s="9"/>
+      <c r="A58" s="6">
+        <v>45190.81372877315</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="3">
+        <v>138308.0</v>
+      </c>
     </row>
     <row r="59">
-      <c r="L59" s="9"/>
+      <c r="A59" s="6">
+        <v>45190.969065625</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="3">
+        <v>137787.0</v>
+      </c>
     </row>
     <row r="60">
-      <c r="L60" s="9"/>
+      <c r="A60" s="6">
+        <v>45194.559409027774</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="3">
+        <v>137776.0</v>
+      </c>
     </row>
     <row r="61">
-      <c r="L61" s="9"/>
+      <c r="A61" s="6">
+        <v>45194.9691953588</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61" s="3">
+        <v>137781.0</v>
+      </c>
     </row>
     <row r="62">
-      <c r="L62" s="9"/>
+      <c r="A62" s="6">
+        <v>45198.853409930554</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="3">
+        <v>138595.0</v>
+      </c>
     </row>
     <row r="63">
-      <c r="L63" s="9"/>
+      <c r="A63" s="6">
+        <v>45202.94876054398</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="3">
+        <v>137983.0</v>
+      </c>
     </row>
     <row r="64">
-      <c r="L64" s="9"/>
+      <c r="A64" s="6">
+        <v>45205.808038958334</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="3">
+        <v>138825.0</v>
+      </c>
     </row>
     <row r="65">
-      <c r="L65" s="9"/>
+      <c r="A65" s="6">
+        <v>45208.34050637731</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="3">
+        <v>140936.0</v>
+      </c>
     </row>
     <row r="66">
-      <c r="L66" s="9"/>
+      <c r="A66" s="6">
+        <v>45209.75382195602</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="3">
+        <v>138300.0</v>
+      </c>
     </row>
     <row r="67">
-      <c r="L67" s="9"/>
+      <c r="A67" s="6">
+        <v>45218.3785619213</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" s="3">
+        <v>138285.0</v>
+      </c>
     </row>
     <row r="68">
-      <c r="L68" s="9"/>
+      <c r="A68" s="6">
+        <v>45218.85161576389</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" s="3">
+        <v>139007.0</v>
+      </c>
     </row>
     <row r="69">
-      <c r="L69" s="9"/>
+      <c r="A69" s="6">
+        <v>45220.87888395833</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69" s="3">
+        <v>138630.0</v>
+      </c>
     </row>
     <row r="70">
-      <c r="L70" s="9"/>
+      <c r="A70" s="6">
+        <v>45228.08618763889</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" s="3">
+        <v>140932.0</v>
+      </c>
     </row>
     <row r="71">
-      <c r="L71" s="9"/>
+      <c r="A71" s="6">
+        <v>45250.50492927083</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="3">
+        <v>138829.0</v>
+      </c>
     </row>
     <row r="72">
-      <c r="L72" s="9"/>
+      <c r="A72" s="6">
+        <v>45250.82424903935</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="3">
+        <v>138827.0</v>
+      </c>
     </row>
     <row r="73">
-      <c r="L73" s="9"/>
+      <c r="A73" s="6">
+        <v>45260.36291415509</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" s="3">
+        <v>141817.0</v>
+      </c>
     </row>
     <row r="74">
-      <c r="L74" s="9"/>
+      <c r="A74" s="6">
+        <v>45260.99141899306</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74" s="3">
+        <v>138826.0</v>
+      </c>
     </row>
     <row r="75">
-      <c r="L75" s="9"/>
+      <c r="A75" s="6">
+        <v>45261.776512743054</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" s="3">
+        <v>140749.0</v>
+      </c>
     </row>
     <row r="76">
-      <c r="L76" s="9"/>
+      <c r="A76" s="6">
+        <v>45263.71840056713</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C76" s="3">
+        <v>140754.0</v>
+      </c>
     </row>
     <row r="77">
-      <c r="L77" s="9"/>
+      <c r="A77" s="6">
+        <v>45268.47352532407</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C77" s="3">
+        <v>140904.0</v>
+      </c>
     </row>
     <row r="78">
-      <c r="L78" s="9"/>
+      <c r="A78" s="6">
+        <v>45268.58581967592</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="3">
+        <v>140903.0</v>
+      </c>
     </row>
     <row r="79">
-      <c r="L79" s="9"/>
+      <c r="A79" s="6">
+        <v>45271.8028274074</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C79" s="3">
+        <v>140914.0</v>
+      </c>
     </row>
     <row r="80">
-      <c r="L80" s="9"/>
+      <c r="A80" s="6"/>
+      <c r="B80" s="3"/>
     </row>
     <row r="81">
+      <c r="K81" s="3"/>
       <c r="L81" s="9"/>
     </row>
     <row r="82">
       <c r="L82" s="9"/>
     </row>
     <row r="83">
+      <c r="K83" s="10"/>
       <c r="L83" s="9"/>
     </row>
     <row r="84">
@@ -2604,6 +4074,117 @@
     </row>
     <row r="142">
       <c r="L142" s="9"/>
+    </row>
+    <row r="143">
+      <c r="L143" s="9"/>
+    </row>
+    <row r="144">
+      <c r="L144" s="9"/>
+    </row>
+    <row r="145">
+      <c r="L145" s="9"/>
+    </row>
+    <row r="146">
+      <c r="L146" s="9"/>
+    </row>
+    <row r="147">
+      <c r="L147" s="9"/>
+    </row>
+    <row r="148">
+      <c r="L148" s="9"/>
+    </row>
+    <row r="149">
+      <c r="L149" s="9"/>
+    </row>
+    <row r="150">
+      <c r="L150" s="9"/>
+    </row>
+    <row r="151">
+      <c r="L151" s="9"/>
+    </row>
+    <row r="152">
+      <c r="L152" s="9"/>
+    </row>
+    <row r="153">
+      <c r="L153" s="9"/>
+    </row>
+    <row r="154">
+      <c r="L154" s="9"/>
+    </row>
+    <row r="155">
+      <c r="L155" s="9"/>
+    </row>
+    <row r="156">
+      <c r="L156" s="9"/>
+    </row>
+    <row r="157">
+      <c r="L157" s="9"/>
+    </row>
+    <row r="158">
+      <c r="L158" s="9"/>
+    </row>
+    <row r="159">
+      <c r="L159" s="9"/>
+    </row>
+    <row r="160">
+      <c r="L160" s="9"/>
+    </row>
+    <row r="161">
+      <c r="L161" s="9"/>
+    </row>
+    <row r="162">
+      <c r="L162" s="9"/>
+    </row>
+    <row r="163">
+      <c r="L163" s="9"/>
+    </row>
+    <row r="164">
+      <c r="L164" s="9"/>
+    </row>
+    <row r="165">
+      <c r="L165" s="9"/>
+    </row>
+    <row r="166">
+      <c r="L166" s="9"/>
+    </row>
+    <row r="167">
+      <c r="L167" s="9"/>
+    </row>
+    <row r="168">
+      <c r="L168" s="9"/>
+    </row>
+    <row r="169">
+      <c r="L169" s="9"/>
+    </row>
+    <row r="170">
+      <c r="L170" s="9"/>
+    </row>
+    <row r="171">
+      <c r="L171" s="9"/>
+    </row>
+    <row r="172">
+      <c r="L172" s="9"/>
+    </row>
+    <row r="173">
+      <c r="L173" s="9"/>
+    </row>
+    <row r="174">
+      <c r="L174" s="9"/>
+    </row>
+    <row r="175">
+      <c r="L175" s="9"/>
+    </row>
+    <row r="176">
+      <c r="L176" s="9"/>
+    </row>
+    <row r="177">
+      <c r="L177" s="9"/>
+    </row>
+    <row r="178">
+      <c r="L178" s="9"/>
+    </row>
+    <row r="179">
+      <c r="L179" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2639,7 +4220,7 @@
   <sheetData>
     <row r="1" ht="31.5" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>104</v>
+        <v>179</v>
       </c>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -2650,34 +4231,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>181</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>107</v>
+        <v>182</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>109</v>
+        <v>184</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>110</v>
+        <v>185</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>111</v>
+        <v>186</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>112</v>
+        <v>187</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>113</v>
+        <v>188</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>114</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3">
@@ -2685,7 +4266,7 @@
         <v>44457.81127759259</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>115</v>
+        <v>190</v>
       </c>
       <c r="C3" s="3">
         <v>5.63</v>
@@ -2694,16 +4275,16 @@
         <v>9.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>116</v>
+        <v>191</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>117</v>
+        <v>192</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>118</v>
+        <v>193</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>119</v>
+        <v>194</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
@@ -2735,7 +4316,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>120</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2">
@@ -2746,28 +4327,28 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>121</v>
+        <v>196</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>197</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>124</v>
+        <v>199</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>125</v>
+        <v>200</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>126</v>
+        <v>201</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>128</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes no laudo, deslocamento da foto do rosto.
</commit_message>
<xml_diff>
--- a/Forms.xlsx
+++ b/Forms.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="211">
   <si>
     <t>PLANILHA DE INFORMAÇÕES GERAIS</t>
   </si>
@@ -521,6 +521,21 @@
   </si>
   <si>
     <t>Sgt. Sebastião</t>
+  </si>
+  <si>
+    <t>0898.9/2023</t>
+  </si>
+  <si>
+    <t>M. Ricardo</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>0869.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Clécio</t>
   </si>
   <si>
     <t>INFORMAÇÕES DAS VÍTIMAS</t>
@@ -2986,7 +3001,53 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="6"/>
+      <c r="A81" s="6">
+        <v>45288.98782309028</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G81" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="6">
+        <v>45289.05578596065</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F82" s="3">
+        <v>1055348.0</v>
+      </c>
+      <c r="G82" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3021,7 +3082,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2">
@@ -3032,37 +3093,37 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3">
@@ -3924,24 +3985,40 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="6"/>
-      <c r="B81" s="3"/>
+      <c r="A81" s="6">
+        <v>45288.98803532407</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C81" s="3">
+        <v>141131.0</v>
+      </c>
     </row>
     <row r="82">
-      <c r="K82" s="3"/>
-      <c r="L82" s="9"/>
+      <c r="A82" s="6">
+        <v>45289.05610061342</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82" s="3">
+        <v>141110.0</v>
+      </c>
     </row>
     <row r="83">
-      <c r="L83" s="9"/>
+      <c r="A83" s="6"/>
+      <c r="B83" s="3"/>
     </row>
     <row r="84">
-      <c r="K84" s="10"/>
+      <c r="K84" s="3"/>
       <c r="L84" s="9"/>
     </row>
     <row r="85">
       <c r="L85" s="9"/>
     </row>
     <row r="86">
+      <c r="K86" s="10"/>
       <c r="L86" s="9"/>
     </row>
     <row r="87">
@@ -4225,6 +4302,12 @@
     </row>
     <row r="180">
       <c r="L180" s="9"/>
+    </row>
+    <row r="181">
+      <c r="L181" s="9"/>
+    </row>
+    <row r="182">
+      <c r="L182" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4260,7 +4343,7 @@
   <sheetData>
     <row r="1" ht="31.5" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -4271,34 +4354,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3">
@@ -4306,7 +4389,7 @@
         <v>44457.81127759259</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C3" s="3">
         <v>5.63</v>
@@ -4315,16 +4398,16 @@
         <v>9.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
@@ -4356,7 +4439,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2">
@@ -4367,28 +4450,28 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exclusão de arquivos desnecessários
</commit_message>
<xml_diff>
--- a/Forms.xlsx
+++ b/Forms.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="240">
   <si>
     <t>PLANILHA DE INFORMAÇÕES GERAIS</t>
   </si>
@@ -536,6 +536,93 @@
   </si>
   <si>
     <t>Sgt. Clécio</t>
+  </si>
+  <si>
+    <t>0878.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Josevaldo</t>
+  </si>
+  <si>
+    <t>0880.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Coelho</t>
+  </si>
+  <si>
+    <t>0894.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Amilton</t>
+  </si>
+  <si>
+    <t>0907.9/2023</t>
+  </si>
+  <si>
+    <t>0924.9/2023</t>
+  </si>
+  <si>
+    <t>PRF Kelson</t>
+  </si>
+  <si>
+    <t>0927.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Túlio Lins</t>
+  </si>
+  <si>
+    <t>0944.9/2023</t>
+  </si>
+  <si>
+    <t>Sd. Queiroz</t>
+  </si>
+  <si>
+    <t>0963.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Arakaty</t>
+  </si>
+  <si>
+    <t>1003.9/2023</t>
+  </si>
+  <si>
+    <t>Cb. Alisson Araujo</t>
+  </si>
+  <si>
+    <t>1017.9/2023</t>
+  </si>
+  <si>
+    <t>Sd. Barros Lima</t>
+  </si>
+  <si>
+    <t>1037.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Lopes</t>
+  </si>
+  <si>
+    <t>1073.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Carlos Lira</t>
+  </si>
+  <si>
+    <t>1075.9/2023</t>
+  </si>
+  <si>
+    <t>xxxxxxxxxxxxxxxxx</t>
+  </si>
+  <si>
+    <t>1076.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Aldivas</t>
+  </si>
+  <si>
+    <t>1086.9/2023</t>
+  </si>
+  <si>
+    <t>Sgt. Amanda Silva</t>
   </si>
   <si>
     <t>INFORMAÇÕES DAS VÍTIMAS</t>
@@ -3047,7 +3134,352 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="6"/>
+      <c r="A83" s="6">
+        <v>45293.86721920139</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F83" s="3">
+        <v>1103911.0</v>
+      </c>
+      <c r="G83" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="6">
+        <v>45293.87013280093</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F84" s="3">
+        <v>9903062.0</v>
+      </c>
+      <c r="G84" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="6">
+        <v>45293.874100671295</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F85" s="3">
+        <v>9802320.0</v>
+      </c>
+      <c r="G85" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="6">
+        <v>45293.87602310185</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F86" s="3">
+        <v>9302930.0</v>
+      </c>
+      <c r="G86" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="6">
+        <v>45293.898267384255</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F87" s="3">
+        <v>1480646.0</v>
+      </c>
+      <c r="G87" s="3">
+        <v>9999999.0</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="6">
+        <v>45293.91707096065</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F88" s="3">
+        <v>1173707.0</v>
+      </c>
+      <c r="G88" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="6">
+        <v>45293.92184587963</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F89" s="3">
+        <v>1253468.0</v>
+      </c>
+      <c r="G89" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="6">
+        <v>45293.930964722225</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F90" s="3">
+        <v>9804579.0</v>
+      </c>
+      <c r="G90" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="6">
+        <v>45294.007446539355</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F91" s="3">
+        <v>1139550.0</v>
+      </c>
+      <c r="G91" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="6">
+        <v>45294.02779574074</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F92" s="3">
+        <v>1085298.0</v>
+      </c>
+      <c r="G92" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="6">
+        <v>45294.308195219906</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F93" s="3">
+        <v>9502629.0</v>
+      </c>
+      <c r="G93" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="6">
+        <v>45294.31335975694</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F94" s="3">
+        <v>9.99999999999E11</v>
+      </c>
+      <c r="G94" s="3">
+        <v>999999.0</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="6">
+        <v>45294.31723011574</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F95" s="3">
+        <v>9.99999999999E11</v>
+      </c>
+      <c r="G95" s="3">
+        <v>9.99999999999E11</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="6">
+        <v>45294.321652025465</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F96" s="3">
+        <v>9802177.0</v>
+      </c>
+      <c r="G96" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="6">
+        <v>45294.32788837963</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F97" s="3">
+        <v>1033000.0</v>
+      </c>
+      <c r="G97" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3082,7 +3514,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
@@ -3093,37 +3525,37 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3">
@@ -4007,66 +4439,194 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="6"/>
-      <c r="B83" s="3"/>
+      <c r="A83" s="6">
+        <v>45293.8675696875</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C83" s="3">
+        <v>141112.0</v>
+      </c>
     </row>
     <row r="84">
-      <c r="K84" s="3"/>
-      <c r="L84" s="9"/>
+      <c r="A84" s="6">
+        <v>45293.870343206014</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C84" s="3">
+        <v>141116.0</v>
+      </c>
     </row>
     <row r="85">
-      <c r="L85" s="9"/>
+      <c r="A85" s="6">
+        <v>45293.87445728009</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="3">
+        <v>141128.0</v>
+      </c>
     </row>
     <row r="86">
-      <c r="K86" s="10"/>
-      <c r="L86" s="9"/>
+      <c r="A86" s="6">
+        <v>45293.87638339121</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C86" s="3">
+        <v>141135.0</v>
+      </c>
     </row>
     <row r="87">
-      <c r="L87" s="9"/>
+      <c r="A87" s="6">
+        <v>45293.89849685185</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C87" s="3">
+        <v>141496.0</v>
+      </c>
     </row>
     <row r="88">
-      <c r="L88" s="9"/>
+      <c r="A88" s="6">
+        <v>45293.91756829861</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C88" s="3">
+        <v>141491.0</v>
+      </c>
     </row>
     <row r="89">
-      <c r="L89" s="9"/>
+      <c r="A89" s="6">
+        <v>45293.922125613426</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C89" s="3">
+        <v>141471.0</v>
+      </c>
     </row>
     <row r="90">
-      <c r="L90" s="9"/>
+      <c r="A90" s="6">
+        <v>45293.931235625</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C90" s="3">
+        <v>141816.0</v>
+      </c>
     </row>
     <row r="91">
-      <c r="L91" s="9"/>
+      <c r="A91" s="6">
+        <v>45294.00795101852</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C91" s="3">
+        <v>141991.0</v>
+      </c>
     </row>
     <row r="92">
-      <c r="L92" s="9"/>
+      <c r="A92" s="6">
+        <v>45294.00834163194</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C92" s="3">
+        <v>142345.0</v>
+      </c>
     </row>
     <row r="93">
-      <c r="L93" s="9"/>
+      <c r="A93" s="6">
+        <v>45294.028106087964</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C93" s="3">
+        <v>141792.0</v>
+      </c>
     </row>
     <row r="94">
-      <c r="L94" s="9"/>
+      <c r="A94" s="6">
+        <v>45294.30866738426</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C94" s="3">
+        <v>142545.0</v>
+      </c>
     </row>
     <row r="95">
-      <c r="L95" s="9"/>
+      <c r="A95" s="6">
+        <v>45294.313720879625</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C95" s="3">
+        <v>142874.0</v>
+      </c>
     </row>
     <row r="96">
-      <c r="L96" s="9"/>
+      <c r="A96" s="6">
+        <v>45294.317430717594</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C96" s="3">
+        <v>142349.0</v>
+      </c>
     </row>
     <row r="97">
-      <c r="L97" s="9"/>
+      <c r="A97" s="6">
+        <v>45294.32205533565</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C97" s="3">
+        <v>142353.0</v>
+      </c>
     </row>
     <row r="98">
-      <c r="L98" s="9"/>
+      <c r="A98" s="6">
+        <v>45294.328089375005</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C98" s="3">
+        <v>142890.0</v>
+      </c>
     </row>
     <row r="99">
-      <c r="L99" s="9"/>
+      <c r="A99" s="6"/>
+      <c r="B99" s="3"/>
     </row>
     <row r="100">
+      <c r="K100" s="3"/>
       <c r="L100" s="9"/>
     </row>
     <row r="101">
       <c r="L101" s="9"/>
     </row>
     <row r="102">
+      <c r="K102" s="10"/>
       <c r="L102" s="9"/>
     </row>
     <row r="103">
@@ -4308,6 +4868,54 @@
     </row>
     <row r="182">
       <c r="L182" s="9"/>
+    </row>
+    <row r="183">
+      <c r="L183" s="9"/>
+    </row>
+    <row r="184">
+      <c r="L184" s="9"/>
+    </row>
+    <row r="185">
+      <c r="L185" s="9"/>
+    </row>
+    <row r="186">
+      <c r="L186" s="9"/>
+    </row>
+    <row r="187">
+      <c r="L187" s="9"/>
+    </row>
+    <row r="188">
+      <c r="L188" s="9"/>
+    </row>
+    <row r="189">
+      <c r="L189" s="9"/>
+    </row>
+    <row r="190">
+      <c r="L190" s="9"/>
+    </row>
+    <row r="191">
+      <c r="L191" s="9"/>
+    </row>
+    <row r="192">
+      <c r="L192" s="9"/>
+    </row>
+    <row r="193">
+      <c r="L193" s="9"/>
+    </row>
+    <row r="194">
+      <c r="L194" s="9"/>
+    </row>
+    <row r="195">
+      <c r="L195" s="9"/>
+    </row>
+    <row r="196">
+      <c r="L196" s="9"/>
+    </row>
+    <row r="197">
+      <c r="L197" s="9"/>
+    </row>
+    <row r="198">
+      <c r="L198" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4343,7 +4951,7 @@
   <sheetData>
     <row r="1" ht="31.5" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -4354,34 +4962,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>189</v>
+        <v>218</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>191</v>
+        <v>220</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>192</v>
+        <v>221</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3">
@@ -4389,7 +4997,7 @@
         <v>44457.81127759259</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>197</v>
+        <v>226</v>
       </c>
       <c r="C3" s="3">
         <v>5.63</v>
@@ -4398,16 +5006,16 @@
         <v>9.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>201</v>
+        <v>230</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
@@ -4439,7 +5047,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2">
@@ -4450,28 +5058,28 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>206</v>
+        <v>235</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizações no texto de LAudo Pericial
Atualizações no texto de LAudo Pericial
</commit_message>
<xml_diff>
--- a/Forms.xlsx
+++ b/Forms.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="121">
   <si>
     <t>PLANILHA DE INFORMAÇÕES GERAIS</t>
   </si>
@@ -257,6 +257,30 @@
   </si>
   <si>
     <t>Sd. Edierck</t>
+  </si>
+  <si>
+    <t>0338.9/2024</t>
+  </si>
+  <si>
+    <t>SGT. BARRETTO</t>
+  </si>
+  <si>
+    <t>0376.9/2024</t>
+  </si>
+  <si>
+    <t>Sgt. P. Cavalcante</t>
+  </si>
+  <si>
+    <t>0382.9/2024</t>
+  </si>
+  <si>
+    <t>Sd. Talles</t>
+  </si>
+  <si>
+    <t>0385.9/2024</t>
+  </si>
+  <si>
+    <t>Cb. Damasceno</t>
   </si>
   <si>
     <t>INFORMAÇÕES DAS VÍTIMAS</t>
@@ -1520,7 +1544,99 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="6"/>
+      <c r="A38" s="6">
+        <v>45415.40557880787</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1104438.0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6">
+        <v>45417.64596840278</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1104870.0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6">
+        <v>45418.577854675925</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1252798.0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6">
+        <v>45418.900479247684</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1182170.0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1555,7 +1671,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
@@ -1566,37 +1682,37 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -1996,30 +2112,62 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="6"/>
-      <c r="B39" s="3"/>
+      <c r="A39" s="6">
+        <v>45415.40603083333</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="3">
+        <v>146204.0</v>
+      </c>
     </row>
     <row r="40">
-      <c r="K40" s="3"/>
-      <c r="L40" s="8"/>
+      <c r="A40" s="6">
+        <v>45417.646333240744</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="3">
+        <v>146212.0</v>
+      </c>
     </row>
     <row r="41">
-      <c r="L41" s="8"/>
+      <c r="A41" s="6">
+        <v>45418.57809548611</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="3">
+        <v>146425.0</v>
+      </c>
     </row>
     <row r="42">
-      <c r="K42" s="9"/>
-      <c r="L42" s="8"/>
+      <c r="A42" s="6">
+        <v>45418.900763784724</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="3">
+        <v>146422.0</v>
+      </c>
     </row>
     <row r="43">
-      <c r="L43" s="8"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="3"/>
     </row>
     <row r="44">
+      <c r="K44" s="3"/>
       <c r="L44" s="8"/>
     </row>
     <row r="45">
       <c r="L45" s="8"/>
     </row>
     <row r="46">
+      <c r="K46" s="9"/>
       <c r="L46" s="8"/>
     </row>
     <row r="47">
@@ -2297,6 +2445,18 @@
     </row>
     <row r="138">
       <c r="L138" s="8"/>
+    </row>
+    <row r="139">
+      <c r="L139" s="8"/>
+    </row>
+    <row r="140">
+      <c r="L140" s="8"/>
+    </row>
+    <row r="141">
+      <c r="L141" s="8"/>
+    </row>
+    <row r="142">
+      <c r="L142" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2332,7 +2492,7 @@
   <sheetData>
     <row r="1" ht="31.5" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -2343,34 +2503,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
@@ -2402,7 +2562,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
@@ -2413,28 +2573,28 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inserção de um instalador precário
</commit_message>
<xml_diff>
--- a/Forms.xlsx
+++ b/Forms.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="302">
   <si>
     <t>PLANILHA DE INFORMAÇÕES GERAIS</t>
   </si>
@@ -514,6 +514,60 @@
     <t>Cb. Norberto</t>
   </si>
   <si>
+    <t>644.9/2024</t>
+  </si>
+  <si>
+    <t>Sgt. Rômulo</t>
+  </si>
+  <si>
+    <t>101.9/2025</t>
+  </si>
+  <si>
+    <t>103.9/2025</t>
+  </si>
+  <si>
+    <t>Sgt. Jânio</t>
+  </si>
+  <si>
+    <t>1.9/2025</t>
+  </si>
+  <si>
+    <t>Sgt. Braga</t>
+  </si>
+  <si>
+    <t>26.9/2025</t>
+  </si>
+  <si>
+    <t>Ten. Jocely</t>
+  </si>
+  <si>
+    <t>111.9/2025</t>
+  </si>
+  <si>
+    <t>837.9/2024</t>
+  </si>
+  <si>
+    <t>Sd. Joanderson</t>
+  </si>
+  <si>
+    <t>918.9/2024</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>12.9/2025</t>
+  </si>
+  <si>
+    <t>Sd. Edimar</t>
+  </si>
+  <si>
+    <t>6.9/2025</t>
+  </si>
+  <si>
+    <t>Sgt. Laurindo</t>
+  </si>
+  <si>
     <t>INFORMAÇÕES DAS VÍTIMAS</t>
   </si>
   <si>
@@ -728,6 +782,84 @@
   </si>
   <si>
     <t>uma sandália azul, com sua tira rompida</t>
+  </si>
+  <si>
+    <t>nenhuma roupa</t>
+  </si>
+  <si>
+    <t>camisa e bermuda multicolores</t>
+  </si>
+  <si>
+    <t>camisa preta e bermuda cinza</t>
+  </si>
+  <si>
+    <t>camisa regata branca e bermuda cinza</t>
+  </si>
+  <si>
+    <t>um par de sandálias de cores branca, preta e vermelha</t>
+  </si>
+  <si>
+    <t>Calvo</t>
+  </si>
+  <si>
+    <t>Camisa azul escuro e bermuda azul claro</t>
+  </si>
+  <si>
+    <t>Arma de fogo, Espingarda</t>
+  </si>
+  <si>
+    <t>camisa vermelha e branca, e bermuda com o nome "Seaway" de cores rosa e cinza</t>
+  </si>
+  <si>
+    <t>um par de sandálias amarelas</t>
+  </si>
+  <si>
+    <t>Espingarda</t>
+  </si>
+  <si>
+    <t>calça com o nome "Seaway" nas cores azul, verde e cinza</t>
+  </si>
+  <si>
+    <t>camisa cinza e bermuda jeans azul</t>
+  </si>
+  <si>
+    <t>um par de sandálias azuis</t>
+  </si>
+  <si>
+    <t>camisa azul e bermuda vermelha</t>
+  </si>
+  <si>
+    <t>um par de sandálias de cores vermelha e preta</t>
+  </si>
+  <si>
+    <t>camisa vermelha e bermuda cinza</t>
+  </si>
+  <si>
+    <t>par de sandálias pretas</t>
+  </si>
+  <si>
+    <t>camisa preta e calça jeans azul</t>
+  </si>
+  <si>
+    <t>bermuda cor bege</t>
+  </si>
+  <si>
+    <t>casaco verde e bermuda rosa, branca e preta, contendo a inscrição "Seaway"</t>
+  </si>
+  <si>
+    <t>lençol</t>
+  </si>
+  <si>
+    <t>camiseta preta e bermuda azul escura</t>
+  </si>
+  <si>
+    <t>uma sandália branca</t>
+  </si>
+  <si>
+    <t>bermuda preta e laranja</t>
+  </si>
+  <si>
+    <t>camiseta cinza e bermuda amarela</t>
   </si>
   <si>
     <t>CADASTRO DE ELEMENTOS BALÍSTICOS</t>
@@ -3084,7 +3216,207 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="8"/>
+      <c r="A80" s="8">
+        <v>45698.84725291667</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F80" s="4">
+        <v>1075268.0</v>
+      </c>
+      <c r="G80" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="8">
+        <v>45698.93731594908</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F81" s="4">
+        <v>1215639.0</v>
+      </c>
+      <c r="G81" s="4">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="8">
+        <v>45699.79927459491</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F82" s="4">
+        <v>9808272.0</v>
+      </c>
+      <c r="G82" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="8">
+        <v>45700.43425503472</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F83" s="4">
+        <v>1047000.0</v>
+      </c>
+      <c r="G83" s="4">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="8">
+        <v>45700.90841769676</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F84" s="4">
+        <v>1041916.0</v>
+      </c>
+      <c r="G84" s="4">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="8">
+        <v>45705.967550092595</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F85" s="4">
+        <v>1130617.0</v>
+      </c>
+      <c r="G85" s="4">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="8">
+        <v>45706.07748634259</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F86" s="4">
+        <v>1258990.0</v>
+      </c>
+      <c r="G86" s="4">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="8">
+        <v>45720.648003090275</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F87" s="4">
+        <v>1.1111111E7</v>
+      </c>
+      <c r="G87" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="8">
+        <v>45722.4475984375</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F88" s="4">
+        <v>1263455.0</v>
+      </c>
+      <c r="G88" s="4">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="8">
+        <v>45722.63606238426</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F89" s="4">
+        <v>1105809.0</v>
+      </c>
+      <c r="G89" s="4">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3116,7 +3448,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2">
@@ -3127,49 +3459,49 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>10</v>
@@ -3187,7 +3519,7 @@
         <v>10</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -3839,16 +4171,16 @@
         <v>147856.0</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62">
@@ -3862,46 +4194,46 @@
         <v>151643.0</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O62" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="P62" s="4" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="Q62" s="4" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63">
@@ -3915,46 +4247,46 @@
         <v>456588.0</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="O63" s="4" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="P63" s="4" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="Q63" s="4" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64">
@@ -3968,46 +4300,46 @@
         <v>151671.0</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="N64" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O64" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="P64" s="4" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="Q64" s="4" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
     </row>
     <row r="65">
@@ -4021,46 +4353,46 @@
         <v>149164.0</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O65" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="P65" s="4" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="Q65" s="4" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
     </row>
     <row r="66">
@@ -4074,46 +4406,46 @@
         <v>151341.0</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="N66" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="O66" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="P66" s="4" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="Q66" s="4" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67">
@@ -4127,46 +4459,46 @@
         <v>148030.0</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="O67" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="P67" s="4" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="Q67" s="4" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68">
@@ -4180,46 +4512,46 @@
         <v>151667.0</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K68" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M68" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="N68" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="N68" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="O68" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="P68" s="4" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="Q68" s="4" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69">
@@ -4233,46 +4565,46 @@
         <v>150546.0</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="N69" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O69" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="P69" s="4" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="Q69" s="4" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
     </row>
     <row r="70">
@@ -4286,46 +4618,46 @@
         <v>152122.0</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K70" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O70" s="4" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="P70" s="4" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="Q70" s="4" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71">
@@ -4339,46 +4671,46 @@
         <v>148031.0</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O71" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="P71" s="4" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="Q71" s="4" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72">
@@ -4392,46 +4724,46 @@
         <v>148037.0</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K72" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O72" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="P72" s="4" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="Q72" s="4" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73">
@@ -4445,46 +4777,46 @@
         <v>148049.0</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="O73" s="4" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="P73" s="4" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="Q73" s="4" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74">
@@ -4498,46 +4830,46 @@
         <v>147847.0</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="F74" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L74" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M74" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N74" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="G74" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="I74" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="J74" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K74" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="L74" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="M74" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="N74" s="4" t="s">
-        <v>210</v>
-      </c>
       <c r="O74" s="4" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="P74" s="4" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="Q74" s="4" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75">
@@ -4551,46 +4883,46 @@
         <v>149170.0</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="O75" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="P75" s="4" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="Q75" s="4" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76">
@@ -4604,46 +4936,46 @@
         <v>149152.0</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O76" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="P76" s="4" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="Q76" s="4" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
     </row>
     <row r="77">
@@ -4657,46 +4989,46 @@
         <v>150587.0</v>
       </c>
       <c r="D77" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L77" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M77" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N77" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="O77" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P77" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q77" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="H77" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="I77" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="K77" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="L77" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="M77" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="N77" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="O77" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="P77" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q77" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="78">
@@ -4710,46 +5042,46 @@
         <v>148025.0</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="O78" s="4" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="P78" s="4" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="Q78" s="4" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
     </row>
     <row r="79">
@@ -4763,57 +5095,958 @@
         <v>148029.0</v>
       </c>
       <c r="D79" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="L79" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M79" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N79" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="O79" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="P79" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q79" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="8">
+        <v>45698.85129236111</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="4">
+        <v>149174.0</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L80" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M80" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="N80" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="O80" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P80" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q80" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="8">
+        <v>45698.93922350694</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C81" s="4">
+        <v>155420.0</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L81" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M81" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N81" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="O81" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P81" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q81" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="8">
+        <v>45699.78237006944</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" s="4">
+        <v>155388.0</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L82" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N82" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O82" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P82" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q82" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="E79" s="4" t="s">
+    </row>
+    <row r="83">
+      <c r="A83" s="8">
+        <v>45700.43592040509</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C83" s="4">
+        <v>154882.0</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E83" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="F79" s="4" t="s">
+      <c r="F83" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="I83" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J83" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K83" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L83" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M83" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N83" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="O83" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="P83" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q83" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="8">
+        <v>45701.06523871528</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" s="4">
+        <v>155101.0</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J84" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="K84" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="L84" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M84" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="G79" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="H79" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="I79" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="J79" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="K79" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="L79" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="M79" s="4" t="s">
+      <c r="N84" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O84" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P84" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q84" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="8">
+        <v>45701.07000515047</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" s="4">
+        <v>155102.0</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K85" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L85" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="N79" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="O79" s="4" t="s">
+      <c r="M85" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N85" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="O85" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P85" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q85" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="8">
+        <v>45701.07177226852</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C86" s="4">
+        <v>155103.0</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L86" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="P79" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q79" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="8"/>
-      <c r="B80" s="4"/>
-    </row>
-    <row r="81">
-      <c r="D81" s="4"/>
-    </row>
-    <row r="83">
-      <c r="D83" s="12"/>
+      <c r="M86" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="N86" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="O86" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P86" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q86" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="8">
+        <v>45701.08622409722</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" s="4">
+        <v>155104.0</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K87" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M87" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N87" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="O87" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="P87" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q87" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="8">
+        <v>45701.089385625004</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C88" s="4">
+        <v>155105.0</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K88" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L88" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M88" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="N88" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O88" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P88" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q88" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="8">
+        <v>45701.09807521991</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" s="4">
+        <v>155106.0</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="K89" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="L89" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M89" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N89" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="O89" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P89" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q89" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="8">
+        <v>45701.10151877315</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C90" s="4">
+        <v>155107.0</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K90" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L90" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="N90" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="O90" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="P90" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q90" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="8">
+        <v>45705.96853336805</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C91" s="4">
+        <v>155407.0</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="K91" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L91" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M91" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="N91" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O91" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P91" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q91" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="8">
+        <v>45705.97003362268</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C92" s="4">
+        <v>155813.0</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="K92" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="L92" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M92" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N92" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="O92" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="P92" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q92" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="8">
+        <v>45706.07874452547</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" s="4">
+        <v>150832.0</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L93" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M93" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="N93" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O93" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P93" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q93" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="8">
+        <v>45720.649509201394</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C94" s="4">
+        <v>151673.0</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I94" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J94" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L94" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N94" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O94" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P94" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q94" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="8">
+        <v>45722.448703587965</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C95" s="4">
+        <v>154894.0</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K95" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L95" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M95" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N95" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="O95" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P95" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q95" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="8">
+        <v>45722.63728730324</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C96" s="4">
+        <v>154896.0</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K96" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L96" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M96" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N96" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O96" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P96" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q96" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="8"/>
+      <c r="B97" s="4"/>
+    </row>
+    <row r="98">
+      <c r="D98" s="4"/>
+    </row>
+    <row r="100">
+      <c r="D100" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4849,7 +6082,7 @@
   <sheetData>
     <row r="1" ht="31.5" customHeight="1">
       <c r="A1" s="13" t="s">
-        <v>238</v>
+        <v>282</v>
       </c>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -4860,34 +6093,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>239</v>
+        <v>283</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>240</v>
+        <v>284</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>241</v>
+        <v>285</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>242</v>
+        <v>286</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>243</v>
+        <v>287</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>244</v>
+        <v>288</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>245</v>
+        <v>289</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>246</v>
+        <v>290</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>248</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3">
@@ -4919,7 +6152,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>249</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2">
@@ -4930,28 +6163,28 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>250</v>
+        <v>294</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>251</v>
+        <v>295</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>252</v>
+        <v>296</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>253</v>
+        <v>297</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>254</v>
+        <v>298</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>255</v>
+        <v>299</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>257</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>